<commit_message>
Include three new surveys
</commit_message>
<xml_diff>
--- a/app/designerFiles/app/config/tables/gps_mop_up/forms/gps_mop_up/gps_mop_up.xlsx
+++ b/app/designerFiles/app/config/tables/gps_mop_up/forms/gps_mop_up/gps_mop_up.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="16440" windowWidth="29040" xWindow="-120" yWindow="-120"/>
+    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15440" windowWidth="13600" xWindow="420" yWindow="460"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="choices" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="181029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -390,20 +390,20 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V98"/>
+  <dimension ref="A1:V100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:G49"/>
+    <sheetView topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10.75" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col bestFit="1" customWidth="1" max="3" min="3" width="11.5"/>
     <col bestFit="1" customWidth="1" max="4" min="4" width="34"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" width="14.625"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" width="14.6640625"/>
     <col bestFit="1" customWidth="1" max="6" min="6" width="10"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" width="21.875"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" width="50.125"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" width="21.83203125"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" width="50.1640625"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -588,7 +588,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>1. What is the name of the person collecting the GPS point?</t>
+          <t>What is the name of the person collecting the GPS point?</t>
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
@@ -858,7 +858,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2. Choose field site</t>
+          <t>Choose field site</t>
         </is>
       </c>
       <c r="I12" t="inlineStr"/>
@@ -1124,7 +1124,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>3. Collect the GPS coordinates</t>
+          <t>Collect the GPS coordinates</t>
         </is>
       </c>
       <c r="I20" t="inlineStr"/>
@@ -1154,17 +1154,17 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>note</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>manual_gps</t>
+          <t>line</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Enter GPS coordinates manually (if necessary)</t>
+          <t>_____________________</t>
         </is>
       </c>
       <c r="I21" t="inlineStr"/>
@@ -1190,17 +1190,17 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>note</t>
+          <t>text</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>line</t>
+          <t>manual_gps</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>_____________________</t>
+          <t>Enter GPS coordinates manually (if necessary)</t>
         </is>
       </c>
       <c r="I22" t="inlineStr"/>
@@ -1223,34 +1223,26 @@
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>GPS_taken</t>
-        </is>
-      </c>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>select_one</t>
+          <t>note</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>GPS_taken</t>
+          <t>line</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>4. If you did not take GPS, please explain why not</t>
+          <t>_____________________</t>
         </is>
       </c>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
-      <c r="L23" s="1" t="inlineStr">
-        <is>
-          <t>Skip if GPS was taken</t>
-        </is>
-      </c>
+      <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr"/>
@@ -1265,24 +1257,36 @@
     <row r="24">
       <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>if</t>
-        </is>
-      </c>
-      <c r="D24" s="5" t="inlineStr">
-        <is>
-          <t>selected(data('GPS_taken'), 'Other')</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>GPS_taken</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>select_one</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>GPS_taken</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>If you did not take GPS, please explain why not</t>
+        </is>
+      </c>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
+      <c r="L24" s="1" t="inlineStr">
+        <is>
+          <t>Skip if GPS was taken</t>
+        </is>
+      </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr"/>
@@ -1297,24 +1301,20 @@
     <row r="25">
       <c r="A25" t="inlineStr"/>
       <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>if</t>
+        </is>
+      </c>
+      <c r="D25" s="5" t="inlineStr">
+        <is>
+          <t>selected(data('GPS_taken'), 'Other')</t>
+        </is>
+      </c>
       <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>text</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>GPS_taken_other</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>If you did not take GPS, please explain why not (other)</t>
-        </is>
-      </c>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
@@ -1333,16 +1333,24 @@
     <row r="26">
       <c r="A26" t="inlineStr"/>
       <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>end if</t>
-        </is>
-      </c>
+      <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>GPS_taken_other</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>If you did not take GPS, please explain why not (other)</t>
+        </is>
+      </c>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
@@ -1361,28 +1369,16 @@
     <row r="27">
       <c r="A27" t="inlineStr"/>
       <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>end if</t>
+        </is>
+      </c>
       <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>GPS_ID</t>
-        </is>
-      </c>
-      <c r="F27" s="1" t="inlineStr">
-        <is>
-          <t>select_one_with_other</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>GPS_ID</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>5. GPS ID (location type)</t>
-        </is>
-      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
@@ -1401,16 +1397,28 @@
     <row r="28">
       <c r="A28" t="inlineStr"/>
       <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>end screen</t>
-        </is>
-      </c>
+      <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>GPS_ID</t>
+        </is>
+      </c>
+      <c r="F28" s="1" t="inlineStr">
+        <is>
+          <t>select_one_with_other</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>GPS_ID</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>GPS ID (location type)</t>
+        </is>
+      </c>
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
@@ -1429,25 +1437,17 @@
     <row r="29">
       <c r="A29" t="inlineStr"/>
       <c r="B29" t="inlineStr"/>
-      <c r="C29" t="inlineStr"/>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>end screen</t>
+        </is>
+      </c>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>log</t>
-        </is>
-      </c>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'GPS_ID',data('GPS_ID')]]))</t>
-        </is>
-      </c>
+      <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
@@ -1481,7 +1481,7 @@
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'GPS_taken_other',data('GPS_taken_other')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'GPS_ID',data('GPS_ID')]]))</t>
         </is>
       </c>
       <c r="J30" t="inlineStr"/>
@@ -1517,7 +1517,7 @@
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'GPS_taken',data('GPS_taken')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'GPS_taken_other',data('GPS_taken_other')]]))</t>
         </is>
       </c>
       <c r="J31" t="inlineStr"/>
@@ -1553,7 +1553,7 @@
       <c r="H32" t="inlineStr"/>
       <c r="I32" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'line',data('line')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'GPS_taken',data('GPS_taken')]]))</t>
         </is>
       </c>
       <c r="J32" t="inlineStr"/>
@@ -1589,7 +1589,7 @@
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'manual_gps',data('manual_gps')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'line',data('line')]]))</t>
         </is>
       </c>
       <c r="J33" t="inlineStr"/>
@@ -1625,7 +1625,7 @@
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'store_gps',data('store_gps')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'manual_gps',data('manual_gps')]]))</t>
         </is>
       </c>
       <c r="J34" t="inlineStr"/>
@@ -1648,10 +1648,22 @@
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>assign</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>log</t>
+        </is>
+      </c>
       <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr"/>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'line',data('line')]]))</t>
+        </is>
+      </c>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
@@ -1672,10 +1684,22 @@
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>assign</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>log</t>
+        </is>
+      </c>
       <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'store_gps',data('store_gps')]]))</t>
+        </is>
+      </c>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
@@ -1693,14 +1717,8 @@
     <row r="37">
       <c r="A37" t="inlineStr"/>
       <c r="B37" t="inlineStr"/>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>if</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>0</v>
-      </c>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
@@ -1726,16 +1744,8 @@
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>extra_question1</t>
-        </is>
-      </c>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr"/>
       <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr"/>
@@ -1755,25 +1765,19 @@
     <row r="39">
       <c r="A39" t="inlineStr"/>
       <c r="B39" t="inlineStr"/>
-      <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr"/>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>if</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
       <c r="E39" t="inlineStr"/>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>log</t>
-        </is>
-      </c>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question1',data('extra_question1')]]))</t>
-        </is>
-      </c>
+      <c r="I39" t="inlineStr"/>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
@@ -1801,7 +1805,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>extra_question2</t>
+          <t>extra_question1</t>
         </is>
       </c>
       <c r="H40" t="inlineStr"/>
@@ -1839,7 +1843,7 @@
       <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question2',data('extra_question2')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question1',data('extra_question1')]]))</t>
         </is>
       </c>
       <c r="J41" t="inlineStr"/>
@@ -1869,7 +1873,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>extra_question3</t>
+          <t>extra_question2</t>
         </is>
       </c>
       <c r="H42" t="inlineStr"/>
@@ -1907,7 +1911,7 @@
       <c r="H43" t="inlineStr"/>
       <c r="I43" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question3',data('extra_question3')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question2',data('extra_question2')]]))</t>
         </is>
       </c>
       <c r="J43" t="inlineStr"/>
@@ -1937,7 +1941,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>extra_question4</t>
+          <t>extra_question3</t>
         </is>
       </c>
       <c r="H44" t="inlineStr"/>
@@ -1975,7 +1979,7 @@
       <c r="H45" t="inlineStr"/>
       <c r="I45" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question4',data('extra_question4')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question3',data('extra_question3')]]))</t>
         </is>
       </c>
       <c r="J45" t="inlineStr"/>
@@ -2005,7 +2009,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>extra_question5</t>
+          <t>extra_question4</t>
         </is>
       </c>
       <c r="H46" t="inlineStr"/>
@@ -2043,7 +2047,7 @@
       <c r="H47" t="inlineStr"/>
       <c r="I47" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question5',data('extra_question5')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question4',data('extra_question4')]]))</t>
         </is>
       </c>
       <c r="J47" t="inlineStr"/>
@@ -2073,7 +2077,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>extra_question6</t>
+          <t>extra_question5</t>
         </is>
       </c>
       <c r="H48" t="inlineStr"/>
@@ -2111,7 +2115,7 @@
       <c r="H49" t="inlineStr"/>
       <c r="I49" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question6',data('extra_question6')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question5',data('extra_question5')]]))</t>
         </is>
       </c>
       <c r="J49" t="inlineStr"/>
@@ -2141,7 +2145,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>extra_question7</t>
+          <t>extra_question6</t>
         </is>
       </c>
       <c r="H50" t="inlineStr"/>
@@ -2179,7 +2183,7 @@
       <c r="H51" t="inlineStr"/>
       <c r="I51" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question7',data('extra_question7')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question6',data('extra_question6')]]))</t>
         </is>
       </c>
       <c r="J51" t="inlineStr"/>
@@ -2209,7 +2213,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>extra_question8</t>
+          <t>extra_question7</t>
         </is>
       </c>
       <c r="H52" t="inlineStr"/>
@@ -2247,7 +2251,7 @@
       <c r="H53" t="inlineStr"/>
       <c r="I53" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question8',data('extra_question8')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question7',data('extra_question7')]]))</t>
         </is>
       </c>
       <c r="J53" t="inlineStr"/>
@@ -2277,7 +2281,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>extra_question9</t>
+          <t>extra_question8</t>
         </is>
       </c>
       <c r="H54" t="inlineStr"/>
@@ -2315,7 +2319,7 @@
       <c r="H55" t="inlineStr"/>
       <c r="I55" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question9',data('extra_question9')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question8',data('extra_question8')]]))</t>
         </is>
       </c>
       <c r="J55" t="inlineStr"/>
@@ -2345,7 +2349,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>extra_question10</t>
+          <t>extra_question9</t>
         </is>
       </c>
       <c r="H56" t="inlineStr"/>
@@ -2383,7 +2387,7 @@
       <c r="H57" t="inlineStr"/>
       <c r="I57" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question10',data('extra_question10')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question9',data('extra_question9')]]))</t>
         </is>
       </c>
       <c r="J57" t="inlineStr"/>
@@ -2413,7 +2417,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>extra_question11</t>
+          <t>extra_question10</t>
         </is>
       </c>
       <c r="H58" t="inlineStr"/>
@@ -2451,7 +2455,7 @@
       <c r="H59" t="inlineStr"/>
       <c r="I59" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question11',data('extra_question11')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question10',data('extra_question10')]]))</t>
         </is>
       </c>
       <c r="J59" t="inlineStr"/>
@@ -2481,7 +2485,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>extra_question12</t>
+          <t>extra_question11</t>
         </is>
       </c>
       <c r="H60" t="inlineStr"/>
@@ -2519,7 +2523,7 @@
       <c r="H61" t="inlineStr"/>
       <c r="I61" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question12',data('extra_question12')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question11',data('extra_question11')]]))</t>
         </is>
       </c>
       <c r="J61" t="inlineStr"/>
@@ -2549,7 +2553,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>extra_question13</t>
+          <t>extra_question12</t>
         </is>
       </c>
       <c r="H62" t="inlineStr"/>
@@ -2587,7 +2591,7 @@
       <c r="H63" t="inlineStr"/>
       <c r="I63" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question13',data('extra_question13')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question12',data('extra_question12')]]))</t>
         </is>
       </c>
       <c r="J63" t="inlineStr"/>
@@ -2617,7 +2621,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>extra_question14</t>
+          <t>extra_question13</t>
         </is>
       </c>
       <c r="H64" t="inlineStr"/>
@@ -2655,7 +2659,7 @@
       <c r="H65" t="inlineStr"/>
       <c r="I65" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question14',data('extra_question14')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question13',data('extra_question13')]]))</t>
         </is>
       </c>
       <c r="J65" t="inlineStr"/>
@@ -2685,7 +2689,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>extra_question15</t>
+          <t>extra_question14</t>
         </is>
       </c>
       <c r="H66" t="inlineStr"/>
@@ -2723,7 +2727,7 @@
       <c r="H67" t="inlineStr"/>
       <c r="I67" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question15',data('extra_question15')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question14',data('extra_question14')]]))</t>
         </is>
       </c>
       <c r="J67" t="inlineStr"/>
@@ -2753,7 +2757,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>extra_question16</t>
+          <t>extra_question15</t>
         </is>
       </c>
       <c r="H68" t="inlineStr"/>
@@ -2791,7 +2795,7 @@
       <c r="H69" t="inlineStr"/>
       <c r="I69" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question16',data('extra_question16')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question15',data('extra_question15')]]))</t>
         </is>
       </c>
       <c r="J69" t="inlineStr"/>
@@ -2821,7 +2825,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>extra_question17</t>
+          <t>extra_question16</t>
         </is>
       </c>
       <c r="H70" t="inlineStr"/>
@@ -2859,7 +2863,7 @@
       <c r="H71" t="inlineStr"/>
       <c r="I71" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question17',data('extra_question17')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question16',data('extra_question16')]]))</t>
         </is>
       </c>
       <c r="J71" t="inlineStr"/>
@@ -2889,7 +2893,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>extra_question18</t>
+          <t>extra_question17</t>
         </is>
       </c>
       <c r="H72" t="inlineStr"/>
@@ -2927,7 +2931,7 @@
       <c r="H73" t="inlineStr"/>
       <c r="I73" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question18',data('extra_question18')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question17',data('extra_question17')]]))</t>
         </is>
       </c>
       <c r="J73" t="inlineStr"/>
@@ -2957,7 +2961,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>extra_question19</t>
+          <t>extra_question18</t>
         </is>
       </c>
       <c r="H74" t="inlineStr"/>
@@ -2995,7 +2999,7 @@
       <c r="H75" t="inlineStr"/>
       <c r="I75" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question19',data('extra_question19')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question18',data('extra_question18')]]))</t>
         </is>
       </c>
       <c r="J75" t="inlineStr"/>
@@ -3025,7 +3029,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>extra_question20</t>
+          <t>extra_question19</t>
         </is>
       </c>
       <c r="H76" t="inlineStr"/>
@@ -3063,7 +3067,7 @@
       <c r="H77" t="inlineStr"/>
       <c r="I77" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question20',data('extra_question20')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question19',data('extra_question19')]]))</t>
         </is>
       </c>
       <c r="J77" t="inlineStr"/>
@@ -3083,15 +3087,19 @@
     <row r="78">
       <c r="A78" t="inlineStr"/>
       <c r="B78" t="inlineStr"/>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>end if</t>
-        </is>
-      </c>
+      <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr"/>
       <c r="E78" t="inlineStr"/>
-      <c r="F78" t="inlineStr"/>
-      <c r="G78" t="inlineStr"/>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>extra_question20</t>
+        </is>
+      </c>
       <c r="H78" t="inlineStr"/>
       <c r="I78" t="inlineStr"/>
       <c r="J78" t="inlineStr"/>
@@ -3121,13 +3129,13 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>log_0</t>
+          <t>log</t>
         </is>
       </c>
       <c r="H79" t="inlineStr"/>
       <c r="I79" t="inlineStr">
         <is>
-          <t>data('log').substring(0,60000) == '' ? ' ' : data('log').substring(0,60000)</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question20',data('extra_question20')]]))</t>
         </is>
       </c>
       <c r="J79" t="inlineStr"/>
@@ -3147,25 +3155,17 @@
     <row r="80">
       <c r="A80" t="inlineStr"/>
       <c r="B80" t="inlineStr"/>
-      <c r="C80" t="inlineStr"/>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>end if</t>
+        </is>
+      </c>
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr"/>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>log_1</t>
-        </is>
-      </c>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr"/>
-      <c r="I80" t="inlineStr">
-        <is>
-          <t>data('log').substring(60000,120000) == '' ? ' ' : data('log').substring(60000,120000)</t>
-        </is>
-      </c>
+      <c r="I80" t="inlineStr"/>
       <c r="J80" t="inlineStr"/>
       <c r="K80" t="inlineStr"/>
       <c r="L80" t="inlineStr"/>
@@ -3193,13 +3193,13 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>log_2</t>
+          <t>log_0</t>
         </is>
       </c>
       <c r="H81" t="inlineStr"/>
       <c r="I81" t="inlineStr">
         <is>
-          <t>data('log').substring(120000,180000) == '' ? ' ' : data('log').substring(120000,180000)</t>
+          <t>data('log').substring(0,60000) == '' ? ' ' : data('log').substring(0,60000)</t>
         </is>
       </c>
       <c r="J81" t="inlineStr"/>
@@ -3229,13 +3229,13 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>log_3</t>
+          <t>log_1</t>
         </is>
       </c>
       <c r="H82" t="inlineStr"/>
       <c r="I82" t="inlineStr">
         <is>
-          <t>data('log').substring(180000,240000) == '' ? ' ' : data('log').substring(180000,240000)</t>
+          <t>data('log').substring(60000,120000) == '' ? ' ' : data('log').substring(60000,120000)</t>
         </is>
       </c>
       <c r="J82" t="inlineStr"/>
@@ -3265,13 +3265,13 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>log_4</t>
+          <t>log_2</t>
         </is>
       </c>
       <c r="H83" t="inlineStr"/>
       <c r="I83" t="inlineStr">
         <is>
-          <t>data('log').substring(240000,300000) == '' ? ' ' : data('log').substring(240000,300000)</t>
+          <t>data('log').substring(120000,180000) == '' ? ' ' : data('log').substring(120000,180000)</t>
         </is>
       </c>
       <c r="J83" t="inlineStr"/>
@@ -3301,13 +3301,13 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>log_5</t>
+          <t>log_3</t>
         </is>
       </c>
       <c r="H84" t="inlineStr"/>
       <c r="I84" t="inlineStr">
         <is>
-          <t>data('log').substring(300000,360000) == '' ? ' ' : data('log').substring(300000,360000)</t>
+          <t>data('log').substring(180000,240000) == '' ? ' ' : data('log').substring(180000,240000)</t>
         </is>
       </c>
       <c r="J84" t="inlineStr"/>
@@ -3337,13 +3337,13 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>log_6</t>
+          <t>log_4</t>
         </is>
       </c>
       <c r="H85" t="inlineStr"/>
       <c r="I85" t="inlineStr">
         <is>
-          <t>data('log').substring(360000,420000) == '' ? ' ' : data('log').substring(360000,420000)</t>
+          <t>data('log').substring(240000,300000) == '' ? ' ' : data('log').substring(240000,300000)</t>
         </is>
       </c>
       <c r="J85" t="inlineStr"/>
@@ -3373,13 +3373,13 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>log_7</t>
+          <t>log_5</t>
         </is>
       </c>
       <c r="H86" t="inlineStr"/>
       <c r="I86" t="inlineStr">
         <is>
-          <t>data('log').substring(420000,480000) == '' ? ' ' : data('log').substring(420000,480000)</t>
+          <t>data('log').substring(300000,360000) == '' ? ' ' : data('log').substring(300000,360000)</t>
         </is>
       </c>
       <c r="J86" t="inlineStr"/>
@@ -3409,13 +3409,13 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>log_8</t>
+          <t>log_6</t>
         </is>
       </c>
       <c r="H87" t="inlineStr"/>
       <c r="I87" t="inlineStr">
         <is>
-          <t>data('log').substring(480000,540000) == '' ? ' ' : data('log').substring(480000,540000)</t>
+          <t>data('log').substring(360000,420000) == '' ? ' ' : data('log').substring(360000,420000)</t>
         </is>
       </c>
       <c r="J87" t="inlineStr"/>
@@ -3445,13 +3445,13 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>log_9</t>
+          <t>log_7</t>
         </is>
       </c>
       <c r="H88" t="inlineStr"/>
       <c r="I88" t="inlineStr">
         <is>
-          <t>data('log').substring(540000,600000) == '' ? ' ' : data('log').substring(540000,600000)</t>
+          <t>data('log').substring(420000,480000) == '' ? ' ' : data('log').substring(420000,480000)</t>
         </is>
       </c>
       <c r="J88" t="inlineStr"/>
@@ -3481,13 +3481,13 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>log_10</t>
+          <t>log_8</t>
         </is>
       </c>
       <c r="H89" t="inlineStr"/>
       <c r="I89" t="inlineStr">
         <is>
-          <t>data('log').substring(600000,660000) == '' ? ' ' : data('log').substring(600000,660000)</t>
+          <t>data('log').substring(480000,540000) == '' ? ' ' : data('log').substring(480000,540000)</t>
         </is>
       </c>
       <c r="J89" t="inlineStr"/>
@@ -3517,13 +3517,13 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>log_11</t>
+          <t>log_9</t>
         </is>
       </c>
       <c r="H90" t="inlineStr"/>
       <c r="I90" t="inlineStr">
         <is>
-          <t>data('log').substring(660000,720000) == '' ? ' ' : data('log').substring(660000,720000)</t>
+          <t>data('log').substring(540000,600000) == '' ? ' ' : data('log').substring(540000,600000)</t>
         </is>
       </c>
       <c r="J90" t="inlineStr"/>
@@ -3553,13 +3553,13 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>log_12</t>
+          <t>log_10</t>
         </is>
       </c>
       <c r="H91" t="inlineStr"/>
       <c r="I91" t="inlineStr">
         <is>
-          <t>data('log').substring(720000,780000) == '' ? ' ' : data('log').substring(720000,780000)</t>
+          <t>data('log').substring(600000,660000) == '' ? ' ' : data('log').substring(600000,660000)</t>
         </is>
       </c>
       <c r="J91" t="inlineStr"/>
@@ -3589,13 +3589,13 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>log_13</t>
+          <t>log_11</t>
         </is>
       </c>
       <c r="H92" t="inlineStr"/>
       <c r="I92" t="inlineStr">
         <is>
-          <t>data('log').substring(780000,840000) == '' ? ' ' : data('log').substring(780000,840000)</t>
+          <t>data('log').substring(660000,720000) == '' ? ' ' : data('log').substring(660000,720000)</t>
         </is>
       </c>
       <c r="J92" t="inlineStr"/>
@@ -3625,13 +3625,13 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>log_14</t>
+          <t>log_12</t>
         </is>
       </c>
       <c r="H93" t="inlineStr"/>
       <c r="I93" t="inlineStr">
         <is>
-          <t>data('log').substring(840000,900000) == '' ? ' ' : data('log').substring(840000,900000)</t>
+          <t>data('log').substring(720000,780000) == '' ? ' ' : data('log').substring(720000,780000)</t>
         </is>
       </c>
       <c r="J93" t="inlineStr"/>
@@ -3661,13 +3661,13 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>log_15</t>
+          <t>log_13</t>
         </is>
       </c>
       <c r="H94" t="inlineStr"/>
       <c r="I94" t="inlineStr">
         <is>
-          <t>data('log').substring(900000,960000) == '' ? ' ' : data('log').substring(900000,960000)</t>
+          <t>data('log').substring(780000,840000) == '' ? ' ' : data('log').substring(780000,840000)</t>
         </is>
       </c>
       <c r="J94" t="inlineStr"/>
@@ -3697,13 +3697,13 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>log_16</t>
+          <t>log_14</t>
         </is>
       </c>
       <c r="H95" t="inlineStr"/>
       <c r="I95" t="inlineStr">
         <is>
-          <t>data('log').substring(960000,1020000) == '' ? ' ' : data('log').substring(960000,1020000)</t>
+          <t>data('log').substring(840000,900000) == '' ? ' ' : data('log').substring(840000,900000)</t>
         </is>
       </c>
       <c r="J95" t="inlineStr"/>
@@ -3733,13 +3733,13 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>log_17</t>
+          <t>log_15</t>
         </is>
       </c>
       <c r="H96" t="inlineStr"/>
       <c r="I96" t="inlineStr">
         <is>
-          <t>data('log').substring(1020000,1080000) == '' ? ' ' : data('log').substring(1020000,1080000)</t>
+          <t>data('log').substring(900000,960000) == '' ? ' ' : data('log').substring(900000,960000)</t>
         </is>
       </c>
       <c r="J96" t="inlineStr"/>
@@ -3769,13 +3769,13 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>log_18</t>
+          <t>log_16</t>
         </is>
       </c>
       <c r="H97" t="inlineStr"/>
       <c r="I97" t="inlineStr">
         <is>
-          <t>data('log').substring(1080000,1140000) == '' ? ' ' : data('log').substring(1080000,1140000)</t>
+          <t>data('log').substring(960000,1020000) == '' ? ' ' : data('log').substring(960000,1020000)</t>
         </is>
       </c>
       <c r="J97" t="inlineStr"/>
@@ -3805,13 +3805,13 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>log_19</t>
+          <t>log_17</t>
         </is>
       </c>
       <c r="H98" t="inlineStr"/>
       <c r="I98" t="inlineStr">
         <is>
-          <t>data('log').substring(1140000,1200000) == '' ? ' ' : data('log').substring(1140000,1200000)</t>
+          <t>data('log').substring(1020000,1080000) == '' ? ' ' : data('log').substring(1020000,1080000)</t>
         </is>
       </c>
       <c r="J98" t="inlineStr"/>
@@ -3827,6 +3827,78 @@
       <c r="T98" t="inlineStr"/>
       <c r="U98" t="inlineStr"/>
       <c r="V98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr"/>
+      <c r="B99" t="inlineStr"/>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr"/>
+      <c r="E99" t="inlineStr"/>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>assign</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>log_18</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr"/>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>data('log').substring(1080000,1140000) == '' ? ' ' : data('log').substring(1080000,1140000)</t>
+        </is>
+      </c>
+      <c r="J99" t="inlineStr"/>
+      <c r="K99" t="inlineStr"/>
+      <c r="L99" t="inlineStr"/>
+      <c r="M99" t="inlineStr"/>
+      <c r="N99" t="inlineStr"/>
+      <c r="O99" t="inlineStr"/>
+      <c r="P99" t="inlineStr"/>
+      <c r="Q99" t="inlineStr"/>
+      <c r="R99" t="inlineStr"/>
+      <c r="S99" t="inlineStr"/>
+      <c r="T99" t="inlineStr"/>
+      <c r="U99" t="inlineStr"/>
+      <c r="V99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr"/>
+      <c r="B100" t="inlineStr"/>
+      <c r="C100" t="inlineStr"/>
+      <c r="D100" t="inlineStr"/>
+      <c r="E100" t="inlineStr"/>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>assign</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>log_19</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr"/>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>data('log').substring(1140000,1200000) == '' ? ' ' : data('log').substring(1140000,1200000)</t>
+        </is>
+      </c>
+      <c r="J100" t="inlineStr"/>
+      <c r="K100" t="inlineStr"/>
+      <c r="L100" t="inlineStr"/>
+      <c r="M100" t="inlineStr"/>
+      <c r="N100" t="inlineStr"/>
+      <c r="O100" t="inlineStr"/>
+      <c r="P100" t="inlineStr"/>
+      <c r="Q100" t="inlineStr"/>
+      <c r="R100" t="inlineStr"/>
+      <c r="S100" t="inlineStr"/>
+      <c r="T100" t="inlineStr"/>
+      <c r="U100" t="inlineStr"/>
+      <c r="V100" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -3845,7 +3917,7 @@
       <selection activeCell="A1" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10.75" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -4273,12 +4345,12 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10.75" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1">
+    <row customHeight="1" ht="28" r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
           <t>setting_name</t>
@@ -4326,7 +4398,7 @@
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5">
@@ -4354,14 +4426,14 @@
   </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10.75" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="14.625"/>
-    <col bestFit="1" customWidth="1" max="3" min="2" width="22.125"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="14.6640625"/>
+    <col bestFit="1" customWidth="1" max="3" min="2" width="22.1640625"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>